<commit_message>
deletar de carros funcionando
</commit_message>
<xml_diff>
--- a/planilhas/motoristas.xlsx
+++ b/planilhas/motoristas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\VoidDash\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B9BC68-162E-4A5D-A1FD-178C25BE4822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE4649A-2E97-4CB2-9755-8E63AAC69368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Luiz Fernando Souza Santos</t>
   </si>
   <si>
-    <t>Guilherme da Silva Cosdta</t>
-  </si>
-  <si>
     <t>Rodrigo Alves Pereira</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>&amp;*DSL784</t>
+  </si>
+  <si>
+    <t>Guilherme da Silva Costa</t>
   </si>
 </sst>
 </file>
@@ -185,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,6 +204,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +524,7 @@
   <dimension ref="A1:GC33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,10 +538,10 @@
   <sheetData>
     <row r="1" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -547,14 +550,14 @@
         <v>0</v>
       </c>
       <c r="GC1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>4512</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5">
@@ -709,7 +712,7 @@
         <v>7468</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5">
         <v>31965662296</v>
@@ -723,7 +726,7 @@
         <v>4456</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5">
         <v>78456298467</v>
@@ -737,7 +740,7 @@
         <v>7784</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="5">
         <v>80283362732</v>
@@ -751,7 +754,7 @@
         <v>9588</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="5">
         <v>57141775530</v>
@@ -765,7 +768,7 @@
         <v>9566</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="5">
         <v>96888892503</v>
@@ -779,7 +782,7 @@
         <v>9531</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5">
         <v>40297476890</v>
@@ -793,7 +796,7 @@
         <v>7585</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5">
         <v>25840445336</v>
@@ -807,7 +810,7 @@
         <v>1264</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="5">
         <v>84840898287</v>
@@ -821,7 +824,7 @@
         <v>4826</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="5">
         <v>59357418184</v>
@@ -835,7 +838,7 @@
         <v>4952</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="5">
         <v>12116893346</v>
@@ -849,7 +852,7 @@
         <v>2477</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="5">
         <v>49096010301</v>
@@ -863,7 +866,7 @@
         <v>4511</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" s="5">
         <v>66353195652</v>
@@ -877,7 +880,7 @@
         <v>112</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="5">
         <v>18223861454</v>
@@ -891,7 +894,7 @@
         <v>3201</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="5">
         <v>18223861454</v>
@@ -905,7 +908,7 @@
         <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="5">
         <v>30853266679</v>
@@ -919,7 +922,7 @@
         <v>4700</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="5">
         <v>52215412200</v>
@@ -933,7 +936,7 @@
         <v>4510</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="5">
         <v>10677877525</v>
@@ -947,7 +950,7 @@
         <v>985</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="5">
         <v>27485169240</v>
@@ -961,7 +964,7 @@
         <v>451</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="5">
         <v>13724009882</v>
@@ -975,7 +978,7 @@
         <v>7638</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="5">
         <v>15896190664</v>
@@ -989,7 +992,7 @@
         <v>7999</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="5">
         <v>16691574097</v>

</xml_diff>